<commit_message>
Yakov update Test Cases structure and Excel data
</commit_message>
<xml_diff>
--- a/src/main/resources/Auto-Exercise.xlsx
+++ b/src/main/resources/Auto-Exercise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ygiterman\IdeaProjects\group-project-automation-exercise\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D379385A-430B-40EF-B155-095A222A931F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F245D3-7C87-4A67-AF88-9168BB8AD3AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="customer" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="307">
   <si>
     <t>Run</t>
   </si>
@@ -789,9 +789,6 @@
     <t>Yakov.Johnsonhotmail.com</t>
   </si>
   <si>
-    <t>Olesya.Willsonhotmail.com</t>
-  </si>
-  <si>
     <t>Mostafa.Kinghotmail.com</t>
   </si>
   <si>
@@ -883,13 +880,88 @@
   </si>
   <si>
     <t>Yakov Johnson</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>bDay</t>
+  </si>
+  <si>
+    <t>bMonth</t>
+  </si>
+  <si>
+    <t>bYear</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>1999</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>1989</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>2001</t>
+  </si>
+  <si>
+    <t>1987</t>
+  </si>
+  <si>
+    <t>1975</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>Mrs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -900,6 +972,19 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -927,7 +1012,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -937,10 +1022,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1218,10 +1306,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D70CD7C-F0F4-40F2-A6D0-E558F7C7E7F1}">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1230,25 +1318,28 @@
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="12.85546875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C1" t="s">
         <v>218</v>
@@ -1256,99 +1347,129 @@
       <c r="D1" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="F1" t="s">
         <v>220</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>221</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>245</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>247</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>236</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>238</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>5</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="T1" t="s">
         <v>244</v>
       </c>
-      <c r="P1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="U1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" t="s">
         <v>277</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="F2" t="s">
         <v>278</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>223</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>227</v>
       </c>
-      <c r="H2" t="s">
-        <v>251</v>
-      </c>
       <c r="I2" t="s">
+        <v>278</v>
+      </c>
+      <c r="J2" t="s">
         <v>239</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="K2" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="L2" t="s">
+        <v>258</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="M2" t="s">
         <v>242</v>
       </c>
-      <c r="M2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="O2" t="s">
-        <v>272</v>
-      </c>
-      <c r="P2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="N2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="T2" t="s">
+        <v>271</v>
+      </c>
+      <c r="U2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C3" t="s">
         <v>230</v>
@@ -1356,44 +1477,59 @@
       <c r="D3" t="s">
         <v>233</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>274</v>
+      <c r="E3" s="5" t="s">
+        <v>305</v>
       </c>
       <c r="F3" t="s">
+        <v>273</v>
+      </c>
+      <c r="G3" t="s">
         <v>223</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>246</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
+        <v>251</v>
+      </c>
+      <c r="J3" t="s">
+        <v>239</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="M3" t="s">
+        <v>242</v>
+      </c>
+      <c r="N3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="T3" t="s">
+        <v>272</v>
+      </c>
+      <c r="U3" t="s">
         <v>252</v>
       </c>
-      <c r="I3" t="s">
-        <v>239</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="L3" t="s">
-        <v>242</v>
-      </c>
-      <c r="M3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="O3" t="s">
-        <v>273</v>
-      </c>
-      <c r="P3" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -1404,51 +1540,66 @@
         <v>222</v>
       </c>
       <c r="D4" t="s">
+        <v>254</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="F4" t="s">
         <v>255</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>223</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>224</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>248</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>239</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>242</v>
       </c>
-      <c r="M4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N4" s="1" t="s">
+      <c r="N4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="O4" t="s">
-        <v>269</v>
-      </c>
-      <c r="P4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="P4" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="T4" t="s">
+        <v>268</v>
+      </c>
+      <c r="U4" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
         <v>55</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C5" t="s">
         <v>228</v>
@@ -1456,49 +1607,64 @@
       <c r="D5" t="s">
         <v>231</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="F5" t="s">
         <v>234</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>223</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>225</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>249</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>239</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>257</v>
-      </c>
       <c r="K5" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="L5" t="s">
+        <v>256</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="M5" t="s">
         <v>242</v>
       </c>
-      <c r="M5" t="s">
-        <v>16</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="O5" t="s">
-        <v>270</v>
-      </c>
-      <c r="P5" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="N5" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="T5" t="s">
+        <v>269</v>
+      </c>
+      <c r="U5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
         <v>55</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C6" t="s">
         <v>229</v>
@@ -1506,44 +1672,60 @@
       <c r="D6" t="s">
         <v>232</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="F6" t="s">
         <v>235</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>223</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>226</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>250</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>239</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="K6" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="L6" t="s">
+        <v>257</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="M6" t="s">
         <v>242</v>
       </c>
-      <c r="M6" t="s">
-        <v>16</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="O6" t="s">
-        <v>271</v>
-      </c>
-      <c r="P6" t="s">
-        <v>253</v>
+      <c r="N6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="T6" t="s">
+        <v>270</v>
+      </c>
+      <c r="U6" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Yakov update Test Cases structure and Excel data 2
</commit_message>
<xml_diff>
--- a/src/main/resources/Auto-Exercise.xlsx
+++ b/src/main/resources/Auto-Exercise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ygiterman\IdeaProjects\group-project-automation-exercise\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F245D3-7C87-4A67-AF88-9168BB8AD3AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4216C300-7A1D-474C-AB4C-36CA47A11085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29955" yWindow="2190" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="customer" sheetId="3" r:id="rId1"/>
@@ -1309,7 +1309,7 @@
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1466,40 +1466,40 @@
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="F3" t="s">
-        <v>273</v>
+        <v>234</v>
       </c>
       <c r="G3" t="s">
         <v>223</v>
       </c>
       <c r="H3" t="s">
-        <v>246</v>
+        <v>225</v>
       </c>
       <c r="I3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="J3" t="s">
         <v>239</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="M3" t="s">
         <v>242</v>
@@ -1508,22 +1508,22 @@
         <v>16</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="T3" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="U3" t="s">
         <v>252</v>
@@ -1534,37 +1534,37 @@
         <v>55</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>279</v>
       </c>
       <c r="C4" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="D4" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>305</v>
       </c>
       <c r="F4" t="s">
-        <v>255</v>
+        <v>273</v>
       </c>
       <c r="G4" t="s">
         <v>223</v>
       </c>
       <c r="H4" t="s">
-        <v>224</v>
+        <v>246</v>
       </c>
       <c r="I4" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="J4" t="s">
         <v>239</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>240</v>
+        <v>259</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>241</v>
+        <v>263</v>
       </c>
       <c r="M4" t="s">
         <v>242</v>
@@ -1573,22 +1573,22 @@
         <v>16</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>243</v>
+        <v>267</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="T4" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="U4" t="s">
         <v>252</v>
@@ -1599,37 +1599,37 @@
         <v>55</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>280</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="D5" t="s">
-        <v>231</v>
+        <v>254</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F5" t="s">
-        <v>234</v>
+        <v>255</v>
       </c>
       <c r="G5" t="s">
         <v>223</v>
       </c>
       <c r="H5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J5" t="s">
         <v>239</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="M5" t="s">
         <v>242</v>
@@ -1638,22 +1638,22 @@
         <v>16</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="T5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="U5" t="s">
         <v>252</v>

</xml_diff>

<commit_message>
Aybars update excel reader Data Driven
</commit_message>
<xml_diff>
--- a/src/main/resources/Auto-Exercise.xlsx
+++ b/src/main/resources/Auto-Exercise.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10514"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ygiterman\IdeaProjects\group-project-automation-exercise\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aybars/IdeaProjects/group-project-automation-exercise/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4216C300-7A1D-474C-AB4C-36CA47A11085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4326FE1B-3FDA-BD4B-9AD4-5B94530CC3AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29955" yWindow="2190" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="customer" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="308">
   <si>
     <t>Run</t>
   </si>
@@ -955,13 +955,16 @@
   </si>
   <si>
     <t>Mrs</t>
+  </si>
+  <si>
+    <t>joseph.greenberg1234@hotmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1012,7 +1015,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1029,6 +1032,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1309,32 +1315,31 @@
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" customWidth="1"/>
+    <col min="6" max="6" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="5.5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="12.85546875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="12.83203125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1399,7 +1404,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1415,8 +1420,8 @@
       <c r="E2" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="F2" t="s">
-        <v>278</v>
+      <c r="F2" s="6" t="s">
+        <v>307</v>
       </c>
       <c r="G2" t="s">
         <v>223</v>
@@ -1464,7 +1469,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -1529,7 +1534,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -1594,7 +1599,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -1659,7 +1664,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -1739,19 +1744,19 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="9" style="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="5.5703125" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="7" max="7" width="5.5" customWidth="1"/>
+    <col min="8" max="8" width="6.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1786,7 +1791,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1821,7 +1826,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1856,7 +1861,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1891,7 +1896,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1926,7 +1931,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1961,7 +1966,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1996,7 +2001,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2031,7 +2036,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2066,7 +2071,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2101,7 +2106,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -2136,7 +2141,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2171,7 +2176,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2206,7 +2211,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -2241,7 +2246,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -2276,7 +2281,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -2311,7 +2316,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -2346,7 +2351,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>55</v>
       </c>
@@ -2381,7 +2386,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -2416,7 +2421,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>55</v>
       </c>
@@ -2451,7 +2456,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>55</v>
       </c>
@@ -2486,7 +2491,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -2521,7 +2526,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -2556,7 +2561,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -2591,7 +2596,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>55</v>
       </c>
@@ -2626,7 +2631,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -2661,7 +2666,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -2696,7 +2701,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>55</v>
       </c>
@@ -2731,7 +2736,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -2766,7 +2771,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -2801,7 +2806,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>55</v>
       </c>
@@ -2836,7 +2841,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>55</v>
       </c>
@@ -2871,7 +2876,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -2906,7 +2911,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>55</v>
       </c>
@@ -2941,7 +2946,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>55</v>
       </c>
@@ -2976,7 +2981,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>55</v>
       </c>
@@ -3011,7 +3016,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>55</v>
       </c>
@@ -3046,7 +3051,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>55</v>
       </c>
@@ -3081,7 +3086,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>55</v>
       </c>
@@ -3116,7 +3121,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>55</v>
       </c>
@@ -3151,7 +3156,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>55</v>
       </c>
@@ -3186,7 +3191,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>55</v>
       </c>
@@ -3221,7 +3226,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>55</v>
       </c>
@@ -3256,7 +3261,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -3291,7 +3296,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>55</v>
       </c>
@@ -3326,7 +3331,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>55</v>
       </c>
@@ -3361,7 +3366,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>55</v>
       </c>
@@ -3396,7 +3401,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>55</v>
       </c>
@@ -3431,7 +3436,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -3466,7 +3471,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>55</v>
       </c>
@@ -3501,7 +3506,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>55</v>
       </c>
@@ -3536,7 +3541,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -3571,7 +3576,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>55</v>
       </c>
@@ -3606,7 +3611,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -3641,7 +3646,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -3676,7 +3681,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -3711,7 +3716,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -3746,7 +3751,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>55</v>
       </c>
@@ -3781,7 +3786,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>55</v>
       </c>
@@ -3816,7 +3821,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>55</v>
       </c>
@@ -3851,7 +3856,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>55</v>
       </c>
@@ -3886,7 +3891,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>55</v>
       </c>
@@ -3921,7 +3926,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>55</v>
       </c>
@@ -3956,7 +3961,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>55</v>
       </c>
@@ -3991,7 +3996,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>55</v>
       </c>
@@ -4026,7 +4031,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>55</v>
       </c>
@@ -4061,7 +4066,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>55</v>
       </c>
@@ -4096,7 +4101,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>55</v>
       </c>
@@ -4131,7 +4136,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>55</v>
       </c>
@@ -4166,7 +4171,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>55</v>
       </c>
@@ -4201,7 +4206,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>55</v>
       </c>
@@ -4236,7 +4241,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>55</v>
       </c>
@@ -4271,7 +4276,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>55</v>
       </c>
@@ -4306,7 +4311,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>55</v>
       </c>
@@ -4341,7 +4346,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>55</v>
       </c>
@@ -4376,7 +4381,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>55</v>
       </c>
@@ -4411,7 +4416,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>55</v>
       </c>
@@ -4446,7 +4451,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>55</v>
       </c>
@@ -4481,7 +4486,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>55</v>
       </c>
@@ -4516,7 +4521,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>55</v>
       </c>
@@ -4551,7 +4556,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="81" spans="1:11">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>55</v>
       </c>
@@ -4586,7 +4591,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="82" spans="1:11">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>55</v>
       </c>
@@ -4621,7 +4626,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="83" spans="1:11">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>55</v>
       </c>
@@ -4656,7 +4661,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="84" spans="1:11">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>55</v>
       </c>
@@ -4691,7 +4696,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="85" spans="1:11">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>55</v>
       </c>
@@ -4726,7 +4731,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="86" spans="1:11">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>55</v>
       </c>
@@ -4761,7 +4766,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="87" spans="1:11">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>55</v>
       </c>
@@ -4796,7 +4801,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="88" spans="1:11">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>55</v>
       </c>
@@ -4831,7 +4836,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="89" spans="1:11">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>55</v>
       </c>
@@ -4866,7 +4871,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="90" spans="1:11">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>55</v>
       </c>
@@ -4901,7 +4906,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="91" spans="1:11">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>55</v>
       </c>
@@ -4936,7 +4941,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="92" spans="1:11">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>55</v>
       </c>
@@ -4971,7 +4976,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="93" spans="1:11">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>55</v>
       </c>
@@ -5006,7 +5011,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="94" spans="1:11">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>55</v>
       </c>
@@ -5041,7 +5046,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="95" spans="1:11">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>55</v>
       </c>
@@ -5076,7 +5081,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="96" spans="1:11">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>55</v>
       </c>
@@ -5111,7 +5116,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="97" spans="1:11">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>55</v>
       </c>
@@ -5146,7 +5151,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="98" spans="1:11">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>55</v>
       </c>
@@ -5181,7 +5186,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="99" spans="1:11">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>55</v>
       </c>
@@ -5216,7 +5221,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="100" spans="1:11">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
Yakov update Test Cases structure and Excel data 3
</commit_message>
<xml_diff>
--- a/src/main/resources/Auto-Exercise.xlsx
+++ b/src/main/resources/Auto-Exercise.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aybars/IdeaProjects/group-project-automation-exercise/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ygiterman\IdeaProjects\group-project-automation-exercise\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4326FE1B-3FDA-BD4B-9AD4-5B94530CC3AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64416368-FECC-438B-AACD-8AAB8A405E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2895" yWindow="1650" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="customer" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="307">
   <si>
     <t>Run</t>
   </si>
@@ -955,16 +955,13 @@
   </si>
   <si>
     <t>Mrs</t>
-  </si>
-  <si>
-    <t>joseph.greenberg1234@hotmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -987,9 +984,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1010,12 +1029,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1025,20 +1047,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1315,31 +1341,32 @@
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5" customWidth="1"/>
-    <col min="6" max="6" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="12.83203125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="12.85546875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1404,42 +1431,42 @@
         <v>253</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>276</v>
+        <v>279</v>
+      </c>
+      <c r="C2" t="s">
+        <v>230</v>
       </c>
       <c r="D2" t="s">
-        <v>277</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>307</v>
+        <v>233</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="F2" t="s">
+        <v>273</v>
       </c>
       <c r="G2" t="s">
         <v>223</v>
       </c>
       <c r="H2" t="s">
-        <v>227</v>
+        <v>246</v>
       </c>
       <c r="I2" t="s">
-        <v>278</v>
+        <v>251</v>
       </c>
       <c r="J2" t="s">
         <v>239</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="M2" t="s">
         <v>242</v>
@@ -1448,63 +1475,63 @@
         <v>16</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>289</v>
+        <v>284</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>292</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="T2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="U2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="C3" t="s">
-        <v>228</v>
+        <v>275</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>276</v>
       </c>
       <c r="D3" t="s">
-        <v>231</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="F3" t="s">
-        <v>234</v>
+        <v>277</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>278</v>
       </c>
       <c r="G3" t="s">
         <v>223</v>
       </c>
       <c r="H3" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="I3" t="s">
-        <v>249</v>
+        <v>278</v>
       </c>
       <c r="J3" t="s">
         <v>239</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="M3" t="s">
         <v>242</v>
@@ -1513,63 +1540,63 @@
         <v>16</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="Q3" s="4" t="s">
-        <v>296</v>
+      <c r="Q3" s="1" t="s">
+        <v>289</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="T3" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="U3" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>55</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D4" t="s">
-        <v>233</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>305</v>
+        <v>231</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>306</v>
       </c>
       <c r="F4" t="s">
-        <v>273</v>
+        <v>234</v>
       </c>
       <c r="G4" t="s">
         <v>223</v>
       </c>
       <c r="H4" t="s">
-        <v>246</v>
+        <v>225</v>
       </c>
       <c r="I4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="J4" t="s">
         <v>239</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="M4" t="s">
         <v>242</v>
@@ -1578,28 +1605,28 @@
         <v>16</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="T4" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="U4" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -1612,7 +1639,7 @@
       <c r="D5" t="s">
         <v>254</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>305</v>
       </c>
       <c r="F5" t="s">
@@ -1664,7 +1691,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -1677,7 +1704,7 @@
       <c r="D6" t="s">
         <v>232</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>305</v>
       </c>
       <c r="F6" t="s">
@@ -1730,9 +1757,12 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{E7EFF9D7-9D75-49CD-9D8A-1F3AB346990E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1744,19 +1774,19 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="9" style="1"/>
-    <col min="4" max="4" width="13.83203125" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" customWidth="1"/>
-    <col min="7" max="7" width="5.5" customWidth="1"/>
-    <col min="8" max="8" width="6.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" customWidth="1"/>
-    <col min="10" max="10" width="18.33203125" customWidth="1"/>
-    <col min="11" max="11" width="8.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1791,7 +1821,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1826,7 +1856,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1861,7 +1891,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1896,7 +1926,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1931,7 +1961,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1966,7 +1996,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -2001,7 +2031,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2036,7 +2066,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2071,7 +2101,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2106,7 +2136,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -2141,7 +2171,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2176,7 +2206,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2211,7 +2241,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -2246,7 +2276,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -2281,7 +2311,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -2316,7 +2346,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -2351,7 +2381,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>55</v>
       </c>
@@ -2386,7 +2416,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -2421,7 +2451,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>55</v>
       </c>
@@ -2456,7 +2486,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>55</v>
       </c>
@@ -2491,7 +2521,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -2526,7 +2556,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -2561,7 +2591,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -2596,7 +2626,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
         <v>55</v>
       </c>
@@ -2631,7 +2661,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -2666,7 +2696,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -2701,7 +2731,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
         <v>55</v>
       </c>
@@ -2736,7 +2766,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -2771,7 +2801,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -2806,7 +2836,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11">
       <c r="A31" t="s">
         <v>55</v>
       </c>
@@ -2841,7 +2871,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11">
       <c r="A32" t="s">
         <v>55</v>
       </c>
@@ -2876,7 +2906,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -2911,7 +2941,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11">
       <c r="A34" t="s">
         <v>55</v>
       </c>
@@ -2946,7 +2976,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11">
       <c r="A35" t="s">
         <v>55</v>
       </c>
@@ -2981,7 +3011,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11">
       <c r="A36" t="s">
         <v>55</v>
       </c>
@@ -3016,7 +3046,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11">
       <c r="A37" t="s">
         <v>55</v>
       </c>
@@ -3051,7 +3081,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11">
       <c r="A38" t="s">
         <v>55</v>
       </c>
@@ -3086,7 +3116,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11">
       <c r="A39" t="s">
         <v>55</v>
       </c>
@@ -3121,7 +3151,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11">
       <c r="A40" t="s">
         <v>55</v>
       </c>
@@ -3156,7 +3186,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11">
       <c r="A41" t="s">
         <v>55</v>
       </c>
@@ -3191,7 +3221,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11">
       <c r="A42" t="s">
         <v>55</v>
       </c>
@@ -3226,7 +3256,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11">
       <c r="A43" t="s">
         <v>55</v>
       </c>
@@ -3261,7 +3291,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -3296,7 +3326,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11">
       <c r="A45" t="s">
         <v>55</v>
       </c>
@@ -3331,7 +3361,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11">
       <c r="A46" t="s">
         <v>55</v>
       </c>
@@ -3366,7 +3396,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11">
       <c r="A47" t="s">
         <v>55</v>
       </c>
@@ -3401,7 +3431,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11">
       <c r="A48" t="s">
         <v>55</v>
       </c>
@@ -3436,7 +3466,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -3471,7 +3501,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11">
       <c r="A50" t="s">
         <v>55</v>
       </c>
@@ -3506,7 +3536,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11">
       <c r="A51" t="s">
         <v>55</v>
       </c>
@@ -3541,7 +3571,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -3576,7 +3606,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11">
       <c r="A53" t="s">
         <v>55</v>
       </c>
@@ -3611,7 +3641,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -3646,7 +3676,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -3681,7 +3711,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -3716,7 +3746,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -3751,7 +3781,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11">
       <c r="A58" t="s">
         <v>55</v>
       </c>
@@ -3786,7 +3816,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11">
       <c r="A59" t="s">
         <v>55</v>
       </c>
@@ -3821,7 +3851,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11">
       <c r="A60" t="s">
         <v>55</v>
       </c>
@@ -3856,7 +3886,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11">
       <c r="A61" t="s">
         <v>55</v>
       </c>
@@ -3891,7 +3921,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11">
       <c r="A62" t="s">
         <v>55</v>
       </c>
@@ -3926,7 +3956,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11">
       <c r="A63" t="s">
         <v>55</v>
       </c>
@@ -3961,7 +3991,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11">
       <c r="A64" t="s">
         <v>55</v>
       </c>
@@ -3996,7 +4026,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11">
       <c r="A65" t="s">
         <v>55</v>
       </c>
@@ -4031,7 +4061,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11">
       <c r="A66" t="s">
         <v>55</v>
       </c>
@@ -4066,7 +4096,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11">
       <c r="A67" t="s">
         <v>55</v>
       </c>
@@ -4101,7 +4131,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11">
       <c r="A68" t="s">
         <v>55</v>
       </c>
@@ -4136,7 +4166,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11">
       <c r="A69" t="s">
         <v>55</v>
       </c>
@@ -4171,7 +4201,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11">
       <c r="A70" t="s">
         <v>55</v>
       </c>
@@ -4206,7 +4236,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11">
       <c r="A71" t="s">
         <v>55</v>
       </c>
@@ -4241,7 +4271,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11">
       <c r="A72" t="s">
         <v>55</v>
       </c>
@@ -4276,7 +4306,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11">
       <c r="A73" t="s">
         <v>55</v>
       </c>
@@ -4311,7 +4341,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11">
       <c r="A74" t="s">
         <v>55</v>
       </c>
@@ -4346,7 +4376,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11">
       <c r="A75" t="s">
         <v>55</v>
       </c>
@@ -4381,7 +4411,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11">
       <c r="A76" t="s">
         <v>55</v>
       </c>
@@ -4416,7 +4446,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11">
       <c r="A77" t="s">
         <v>55</v>
       </c>
@@ -4451,7 +4481,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11">
       <c r="A78" t="s">
         <v>55</v>
       </c>
@@ -4486,7 +4516,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11">
       <c r="A79" t="s">
         <v>55</v>
       </c>
@@ -4521,7 +4551,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11">
       <c r="A80" t="s">
         <v>55</v>
       </c>
@@ -4556,7 +4586,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11">
       <c r="A81" t="s">
         <v>55</v>
       </c>
@@ -4591,7 +4621,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11">
       <c r="A82" t="s">
         <v>55</v>
       </c>
@@ -4626,7 +4656,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11">
       <c r="A83" t="s">
         <v>55</v>
       </c>
@@ -4661,7 +4691,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11">
       <c r="A84" t="s">
         <v>55</v>
       </c>
@@ -4696,7 +4726,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11">
       <c r="A85" t="s">
         <v>55</v>
       </c>
@@ -4731,7 +4761,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11">
       <c r="A86" t="s">
         <v>55</v>
       </c>
@@ -4766,7 +4796,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11">
       <c r="A87" t="s">
         <v>55</v>
       </c>
@@ -4801,7 +4831,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11">
       <c r="A88" t="s">
         <v>55</v>
       </c>
@@ -4836,7 +4866,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11">
       <c r="A89" t="s">
         <v>55</v>
       </c>
@@ -4871,7 +4901,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11">
       <c r="A90" t="s">
         <v>55</v>
       </c>
@@ -4906,7 +4936,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11">
       <c r="A91" t="s">
         <v>55</v>
       </c>
@@ -4941,7 +4971,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11">
       <c r="A92" t="s">
         <v>55</v>
       </c>
@@ -4976,7 +5006,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11">
       <c r="A93" t="s">
         <v>55</v>
       </c>
@@ -5011,7 +5041,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11">
       <c r="A94" t="s">
         <v>55</v>
       </c>
@@ -5046,7 +5076,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11">
       <c r="A95" t="s">
         <v>55</v>
       </c>
@@ -5081,7 +5111,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11">
       <c r="A96" t="s">
         <v>55</v>
       </c>
@@ -5116,7 +5146,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11">
       <c r="A97" t="s">
         <v>55</v>
       </c>
@@ -5151,7 +5181,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11">
       <c r="A98" t="s">
         <v>55</v>
       </c>
@@ -5186,7 +5216,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11">
       <c r="A99" t="s">
         <v>55</v>
       </c>
@@ -5221,7 +5251,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11">
       <c r="A100" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
Yakov updated Base Page, completed 10, and 11.  Extended all pages to BasePage
</commit_message>
<xml_diff>
--- a/src/main/resources/Auto-Exercise.xlsx
+++ b/src/main/resources/Auto-Exercise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ygiterman\IdeaProjects\group-project-automation-exercise\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64416368-FECC-438B-AACD-8AAB8A405E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA9770D-22A4-4A59-BEA8-0D72631612F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2895" yWindow="1650" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="customer" sheetId="3" r:id="rId1"/>
@@ -1341,7 +1341,7 @@
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1498,7 +1498,7 @@
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>275</v>

</xml_diff>